<commit_message>
20230612| registro de avances
</commit_message>
<xml_diff>
--- a/personalAccounts/task_bomsai/Bomsai.xlsx
+++ b/personalAccounts/task_bomsai/Bomsai.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>registro</t>
   </si>
@@ -29,21 +29,19 @@
   <si>
     <t>COPROSMA ROJA</t>
   </si>
+  <si>
+    <t>se ponen las hojas negras</t>
+  </si>
+  <si>
+    <t>sequia de hojas luego de riesgo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -74,7 +72,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -393,18 +391,27 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
+        <v>45071</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <v>45085</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>45089</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
@@ -460,7 +467,11 @@
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
     </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>